<commit_message>
added more part numbers to spreadsheet
</commit_message>
<xml_diff>
--- a/common-parts.xlsx
+++ b/common-parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Passives" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="247">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -107,6 +107,27 @@
     <t xml:space="preserve">C1653</t>
   </si>
   <si>
+    <t xml:space="preserve">Cap Tant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_Tantalum_SMD:CP_EIA-3216-10_Kemet-I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLJA107M010R1400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">478-5651-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C313517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
@@ -167,6 +188,30 @@
     <t xml:space="preserve">C203424</t>
   </si>
   <si>
+    <t xml:space="preserve">1K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-JW-102ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-JW-102ELFCT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C118155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-JW-471ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-JW-471ELFCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C169259</t>
+  </si>
+  <si>
     <t xml:space="preserve">100K</t>
   </si>
   <si>
@@ -209,6 +254,18 @@
     <t xml:space="preserve">C12028</t>
   </si>
   <si>
+    <t xml:space="preserve">Resistor_SMD:R_Array_Convex_4x0604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAY16-103J4LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAY16-103J4LFCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C107374</t>
+  </si>
+  <si>
     <t xml:space="preserve">Polyfuse</t>
   </si>
   <si>
@@ -299,6 +356,45 @@
     <t xml:space="preserve">Korean Hroparts Elec</t>
   </si>
   <si>
+    <t xml:space="preserve">Tactile Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">josh-buttons-switches:SW_PUSH_KMR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMR221GLFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401-1427-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C72443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C&amp;K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic substitute okay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">josh-buttons-switches:SW_PUSH_PTS645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS645SL50SMTR92 LFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CKN9088CT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C221877</t>
+  </si>
+  <si>
     <t xml:space="preserve">Microcontroller</t>
   </si>
   <si>
@@ -356,7 +452,7 @@
     <t xml:space="preserve">AP2112K-3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">SOT23-5</t>
+    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-5</t>
   </si>
   <si>
     <t xml:space="preserve">AP2112K-3.3TRG1</t>
@@ -371,6 +467,57 @@
     <t xml:space="preserve">Diodes Inc</t>
   </si>
   <si>
+    <t xml:space="preserve">USB UART Converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP2102N-A01-GQFN28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_DFN_QFN:QFN-28-1EP_5x5mm_P0.5mm_EP3.35x3.35mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">336-4738-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C105167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicon Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH340G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_SO:SOIC-16_3.9x9.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WCH(Jiangsu Qin Heng)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure G variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP8266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP-12F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh-module:ESP-12E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C82891</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ai-Thinker</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED</t>
   </si>
   <si>
@@ -452,9 +599,6 @@
     <t xml:space="preserve">296-25216-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Texas Instruments</t>
   </si>
   <si>
@@ -570,6 +714,57 @@
   </si>
   <si>
     <t xml:space="preserve">490-9647-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THT Piezo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buzzer_Beeper:Buzzer_12x9.5RM7.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMB12A05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C96093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jiangsu Huaneng Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dual NPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-363_SC-70-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBT3904DW1T3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBT3904DW1T3GOSCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C110150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCSC MPN may be incorrect – ensure SOT-363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8 TFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh-display_1.8TFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8" SPI TFT display, 160x128 18-bit color - ST7735R driver (Same as Adafruit PID 618)</t>
   </si>
 </sst>
 </file>
@@ -670,17 +865,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.35"/>
@@ -808,6 +1003,9 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="1"/>
+    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>27</v>
@@ -824,242 +1022,343 @@
       <c r="E7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="G10" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>34</v>
+      <c r="C12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>33</v>
+      <c r="B19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>74</v>
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>78</v>
+        <v>40</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1078,19 +1377,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.11"/>
@@ -1124,48 +1423,100 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>85</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1184,21 +1535,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.38"/>
   </cols>
   <sheetData>
@@ -1230,94 +1581,166 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1339,10 +1762,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.74"/>
@@ -1382,175 +1805,175 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>129</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>136</v>
+        <v>185</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>140</v>
+        <v>189</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>140</v>
+        <v>189</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>157</v>
+        <v>205</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1569,21 +1992,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,97 +2031,172 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>161</v>
+        <v>209</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>163</v>
+        <v>211</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>161</v>
+        <v>209</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>170</v>
+        <v>218</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>173</v>
+        <v>221</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>177</v>
+        <v>225</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>180</v>
+        <v>228</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>78</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "update parts list"
This reverts commit f35513e2f744ac905515b2d09bfaf2a233ce054c.
</commit_message>
<xml_diff>
--- a/common-parts.xlsx
+++ b/common-parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Passives" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="182">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bel Fuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">501mA</t>
   </si>
   <si>
     <t xml:space="preserve">josh-passives-smt:Fuse_0603_1608Metric</t>
@@ -669,11 +672,11 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.49"/>
@@ -1018,19 +1021,19 @@
         <v>61</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>33</v>
@@ -1038,25 +1041,25 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1077,11 +1080,11 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.2"/>
@@ -1121,48 +1124,48 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1183,11 +1186,11 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
@@ -1227,94 +1230,94 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1336,10 +1339,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.74"/>
@@ -1379,175 +1382,175 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1569,10 +1572,10 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.65"/>
@@ -1608,94 +1611,94 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>